<commit_message>
modification to DHFR kinetics excel table
</commit_message>
<xml_diff>
--- a/Tables/Table1_DHFRkinetics.xlsx
+++ b/Tables/Table1_DHFRkinetics.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimreynol/Documents/Projects/DHFRTSEpi/DHFRTSSatMut/2021_AnalysiswTNN/DHTS_EpiAnalysis/Tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimreynol/Documents/Projects/DHFRTSEpi/DHFRTSSatMut/2021_AnalysiswTNN/dhfr-tyms-epistasis/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1306BB73-93AE-EB4D-BD26-A5F549E0B4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF66703-C1C3-F84F-87DE-DA917267EEB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57520" yWindow="4180" windowWidth="27640" windowHeight="16340" xr2:uid="{3C75B9B6-7487-2945-B4A5-C560ADF88E59}"/>
+    <workbookView xWindow="1700" yWindow="660" windowWidth="20820" windowHeight="16500" xr2:uid="{3C75B9B6-7487-2945-B4A5-C560ADF88E59}"/>
   </bookViews>
   <sheets>
     <sheet name="kinetics_dhfr" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">kinetics_dhfr!$A$1:$E$16</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">kinetics_dhfr!$A$1:$E$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t>Mutant</t>
   </si>
@@ -140,6 +140,21 @@
   </si>
   <si>
     <t>Thompson et al. Elife 2020</t>
+  </si>
+  <si>
+    <t>E17V</t>
+  </si>
+  <si>
+    <t>I5K</t>
+  </si>
+  <si>
+    <t>V13H</t>
+  </si>
+  <si>
+    <t>M20Q</t>
+  </si>
+  <si>
+    <t>This work</t>
   </si>
 </sst>
 </file>
@@ -282,6 +297,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -310,7 +326,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -341,15 +356,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D7475A9-E3DB-9344-82BD-6E87F66FC759}" name="kinetics_dhfr" displayName="kinetics_dhfr" ref="A1:F16" tableType="queryTable" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:F16" xr:uid="{2D7475A9-E3DB-9344-82BD-6E87F66FC759}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D7475A9-E3DB-9344-82BD-6E87F66FC759}" name="kinetics_dhfr" displayName="kinetics_dhfr" ref="A1:F20" tableType="queryTable" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F20" xr:uid="{2D7475A9-E3DB-9344-82BD-6E87F66FC759}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{71BFD3F5-D7F4-9541-9268-EA4578021C53}" uniqueName="1" name="DHFR mutation" queryTableFieldId="1" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{73866437-77CD-1C45-AF2E-887E47066BFA}" uniqueName="2" name="kcat" queryTableFieldId="2" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{343383DB-166C-C84A-846D-116C5E3FC9BB}" uniqueName="3" name="Km" queryTableFieldId="3" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{0E5098CA-2240-E54C-8B7F-32CC257DEB65}" uniqueName="4" name="kcat_std" queryTableFieldId="4" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{6DF37569-5829-0247-808B-B70D04404661}" uniqueName="5" name="Km_std" queryTableFieldId="5" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{84CC9F4F-4FC0-884D-AE0B-DFB7C36D403A}" uniqueName="6" name="Reference" queryTableFieldId="6" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{71BFD3F5-D7F4-9541-9268-EA4578021C53}" uniqueName="1" name="DHFR mutation" queryTableFieldId="1" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{73866437-77CD-1C45-AF2E-887E47066BFA}" uniqueName="2" name="kcat" queryTableFieldId="2" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{343383DB-166C-C84A-846D-116C5E3FC9BB}" uniqueName="3" name="Km" queryTableFieldId="3" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{0E5098CA-2240-E54C-8B7F-32CC257DEB65}" uniqueName="4" name="kcat_std" queryTableFieldId="4" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{6DF37569-5829-0247-808B-B70D04404661}" uniqueName="5" name="Km_std" queryTableFieldId="5" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{84CC9F4F-4FC0-884D-AE0B-DFB7C36D403A}" uniqueName="6" name="Reference" queryTableFieldId="6" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -652,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A79AB2-C6CF-D745-93CC-A8704EA72593}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -986,6 +1001,86 @@
       </c>
       <c r="F16" s="1" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>62</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2.85</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>